<commit_message>
Add tags to complete the training set
</commit_message>
<xml_diff>
--- a/VA102_worklog.xlsx
+++ b/VA102_worklog.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>Read about NLTK classifier and look at already existing classifiers</t>
+  </si>
+  <si>
+    <t>Set up git repository</t>
+  </si>
+  <si>
+    <t>Make training and test data set to make the classifier</t>
   </si>
 </sst>
 </file>
@@ -496,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,6 +837,28 @@
       </c>
       <c r="C31" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>42341</v>
+      </c>
+      <c r="B32">
+        <v>0.5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>42355</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>